<commit_message>
update geopandas notebook and geolinking results
</commit_message>
<xml_diff>
--- a/geolinking_results.xlsx
+++ b/geolinking_results.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baselshbita/repos/linked-maps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65249A70-A048-234B-8F2C-2EA4D85DC3C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9E8D92-545E-F84A-8917-6DEF47F76140}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41320" yWindow="740" windowWidth="28120" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5480" yWindow="460" windowWidth="28120" windowHeight="18400" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bray_baseline" sheetId="1" r:id="rId1"/>
-    <sheet name="louisville_baseline" sheetId="3" r:id="rId2"/>
+    <sheet name="bray_lm" sheetId="4" r:id="rId2"/>
+    <sheet name="louisville_baseline" sheetId="3" r:id="rId3"/>
+    <sheet name="louisville_lm" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="58">
   <si>
     <t>GID</t>
   </si>
@@ -201,7 +203,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +222,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -270,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -281,6 +291,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,7 +596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2029,6 +2040,299 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69FF253A-9099-F948-A118-44C7DA0ACDCE}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" customWidth="1"/>
+    <col min="4" max="4" width="36.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7477B414-9C0A-CF44-AC3F-E43BB40B0ADF}">
   <dimension ref="A1:E12"/>
   <sheetViews>
@@ -2251,4 +2555,144 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2BF4B40-4DF4-3242-9CBC-A5AE2E4C1E28}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" customWidth="1"/>
+    <col min="4" max="4" width="36.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update final geolinking results
</commit_message>
<xml_diff>
--- a/geolinking_results.xlsx
+++ b/geolinking_results.xlsx
@@ -8,22 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baselshbita/repos/linked-maps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9E8D92-545E-F84A-8917-6DEF47F76140}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D358ECD0-191A-584F-ABFD-E6FDCF8DAB22}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5480" yWindow="460" windowWidth="28120" windowHeight="18400" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5480" yWindow="460" windowWidth="21260" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="bray_baseline" sheetId="1" r:id="rId1"/>
-    <sheet name="bray_lm" sheetId="4" r:id="rId2"/>
-    <sheet name="louisville_baseline" sheetId="3" r:id="rId3"/>
-    <sheet name="louisville_lm" sheetId="5" r:id="rId4"/>
+    <sheet name="Summary" sheetId="6" r:id="rId1"/>
+    <sheet name="bray_baseline" sheetId="1" r:id="rId2"/>
+    <sheet name="bray_lm" sheetId="4" r:id="rId3"/>
+    <sheet name="bray__recall " sheetId="8" r:id="rId4"/>
+    <sheet name="louisville_baseline" sheetId="3" r:id="rId5"/>
+    <sheet name="louisville_lm" sheetId="5" r:id="rId6"/>
+    <sheet name="louisville__recall" sheetId="9" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'bray__recall '!$A$1:$C$17</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="70">
   <si>
     <t>GID</t>
   </si>
@@ -197,12 +203,51 @@
   </si>
   <si>
     <t>http://linkedmaps.isi.edu/8</t>
+  </si>
+  <si>
+    <t>Bray</t>
+  </si>
+  <si>
+    <t>Louisville</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Bray-baseline</t>
+  </si>
+  <si>
+    <t>Louisville-baseline</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>LM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -232,15 +277,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -276,11 +333,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -291,7 +357,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,6 +667,147 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDCD1294-7A31-704D-92C8-A1212033E5A5}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="3.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2">
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <v>67</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="10">
+        <f>B2/(B2+C2)</f>
+        <v>0.19277108433734941</v>
+      </c>
+      <c r="F2" s="10">
+        <f>B2/(B2+D2)</f>
+        <v>1</v>
+      </c>
+      <c r="G2" s="10">
+        <f>2*E2*F2/(E2+F2)</f>
+        <v>0.32323232323232326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3" s="10">
+        <f t="shared" ref="E3:E5" si="0">B3/(B3+C3)</f>
+        <v>0.8</v>
+      </c>
+      <c r="F3" s="10">
+        <f t="shared" ref="F3:F5" si="1">B3/(B3+D3)</f>
+        <v>0.75</v>
+      </c>
+      <c r="G3" s="10">
+        <f>2*E3*F3/(E3+F3)</f>
+        <v>0.77419354838709686</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10">
+        <f t="shared" si="0"/>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="F4" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G4" s="10">
+        <f t="shared" ref="G4:G5" si="2">2*E4*F4/(E4+F4)</f>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="10">
+        <f t="shared" si="0"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F5" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G5" s="10">
+        <f t="shared" si="2"/>
+        <v>0.90909090909090906</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E84"/>
   <sheetViews>
@@ -2039,13 +2254,610 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69FF253A-9099-F948-A118-44C7DA0ACDCE}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" customWidth="1"/>
+    <col min="4" max="4" width="36.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61067EFA-797E-564B-B635-A89D08761677}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7477B414-9C0A-CF44-AC3F-E43BB40B0ADF}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2074,13 +2886,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -2091,13 +2903,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -2108,30 +2920,30 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -2142,33 +2954,33 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -2176,30 +2988,30 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -2210,33 +3022,33 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2244,87 +3056,19 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2332,13 +3076,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7477B414-9C0A-CF44-AC3F-E43BB40B0ADF}">
-  <dimension ref="A1:E12"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2BF4B40-4DF4-3242-9CBC-A5AE2E4C1E28}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2369,7 +3111,7 @@
       <c r="A2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C2" t="s">
@@ -2378,7 +3120,7 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2386,7 +3128,7 @@
       <c r="A3" t="s">
         <v>40</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C3" t="s">
@@ -2395,7 +3137,7 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2403,25 +3145,25 @@
       <c r="A4" t="s">
         <v>40</v>
       </c>
-      <c r="B4" t="s">
-        <v>43</v>
+      <c r="B4" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="E4" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>40</v>
       </c>
-      <c r="B5" t="s">
-        <v>44</v>
+      <c r="B5" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="C5" t="s">
         <v>48</v>
@@ -2429,15 +3171,15 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5">
-        <v>1</v>
+      <c r="E5" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C6" t="s">
@@ -2446,110 +3188,25 @@
       <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="E6">
-        <v>0</v>
+      <c r="E6" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
+        <v>54</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="E7" s="9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2557,23 +3214,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2BF4B40-4DF4-3242-9CBC-A5AE2E4C1E28}">
-  <dimension ref="A1:E7"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D621577-2121-6A4D-924E-3CC05E98D1C2}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.5" customWidth="1"/>
     <col min="2" max="2" width="39.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.6640625" customWidth="1"/>
-    <col min="4" max="4" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2583,14 +3237,14 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -2600,14 +3254,14 @@
       <c r="C2" t="s">
         <v>48</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -2617,14 +3271,14 @@
       <c r="C3" t="s">
         <v>48</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
       <c r="E3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -2634,61 +3288,44 @@
       <c r="C4" t="s">
         <v>48</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
       <c r="E4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7">
+      <c r="F6">
         <v>1</v>
       </c>
     </row>

</xml_diff>